<commit_message>
Completed the implementation of S3 upload for excel sheet produced by price tracking API and changed column names to the desired format
</commit_message>
<xml_diff>
--- a/excel_sheets/output.xlsx
+++ b/excel_sheets/output.xlsx
@@ -405,31 +405,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>product_id</v>
+        <v>Product Id</v>
       </c>
       <c r="B1" t="str">
-        <v>product_name</v>
+        <v>Product Name</v>
       </c>
       <c r="C1" t="str">
-        <v>current_quantity</v>
+        <v>Current Quantity</v>
       </c>
       <c r="D1" t="str">
-        <v>latest_supplier_name</v>
+        <v>Latest Supplier Name</v>
       </c>
       <c r="E1" t="str">
-        <v>latest_supplier_unit_price</v>
+        <v>Latest Supplier Unit Price</v>
       </c>
       <c r="F1" t="str">
-        <v>latest_supplier_date</v>
+        <v>Latest Supplier Date</v>
       </c>
       <c r="G1" t="str">
-        <v>min_supplier_name</v>
+        <v>Minimum Supplier Name</v>
       </c>
       <c r="H1" t="str">
-        <v>min_supplier_unit_price</v>
+        <v>Minimum Supplier Unit Price</v>
       </c>
       <c r="I1" t="str">
-        <v>min_supplier_date</v>
+        <v>Minimum Supplier Date</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
Added previous to latest supplier query and also corrected removal of customer_id from one month previous min price supplier query
</commit_message>
<xml_diff>
--- a/excel_sheets/output.xlsx
+++ b/excel_sheets/output.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -423,12 +423,21 @@
         <v>Latest Supplier Date</v>
       </c>
       <c r="G1" t="str">
+        <v>Prev Supplier Name</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Prev Supplier Unit Price</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Prev Supplier Date</v>
+      </c>
+      <c r="J1" t="str">
         <v>Minimum Supplier Name</v>
       </c>
-      <c r="H1" t="str">
+      <c r="K1" t="str">
         <v>Minimum Supplier Unit Price</v>
       </c>
-      <c r="I1" t="str">
+      <c r="L1" t="str">
         <v>Minimum Supplier Date</v>
       </c>
     </row>
@@ -443,21 +452,30 @@
         <v>9.00</v>
       </c>
       <c r="D2" t="str">
-        <v>supplier_3</v>
+        <v>supplier_2</v>
       </c>
       <c r="E2" t="str">
+        <v>30.00</v>
+      </c>
+      <c r="F2" s="1">
+        <v>45069.645949074074</v>
+      </c>
+      <c r="G2" t="str">
+        <v>supplier_1</v>
+      </c>
+      <c r="H2" t="str">
         <v>50.00</v>
       </c>
-      <c r="F2" s="1">
-        <v>45069.645949074074</v>
-      </c>
-      <c r="G2" t="str">
+      <c r="I2" s="1">
+        <v>45069.645949074074</v>
+      </c>
+      <c r="J2" t="str">
         <v>supplier_2</v>
       </c>
-      <c r="H2" t="str">
+      <c r="K2" t="str">
         <v>30.00</v>
       </c>
-      <c r="I2" s="1">
+      <c r="L2" s="1">
         <v>45069.645949074074</v>
       </c>
     </row>
@@ -481,12 +499,21 @@
         <v>45069.645949074074</v>
       </c>
       <c r="G3" t="str">
+        <v/>
+      </c>
+      <c r="H3" t="str">
+        <v/>
+      </c>
+      <c r="I3" t="str">
+        <v/>
+      </c>
+      <c r="J3" t="str">
         <v>supplier_1</v>
       </c>
-      <c r="H3" t="str">
+      <c r="K3" t="str">
         <v>50.00</v>
       </c>
-      <c r="I3" s="1">
+      <c r="L3" s="1">
         <v>45069.645949074074</v>
       </c>
     </row>
@@ -510,12 +537,21 @@
         <v>45069.645949074074</v>
       </c>
       <c r="G4" t="str">
+        <v/>
+      </c>
+      <c r="H4" t="str">
+        <v/>
+      </c>
+      <c r="I4" t="str">
+        <v/>
+      </c>
+      <c r="J4" t="str">
         <v>supplier_1</v>
       </c>
-      <c r="H4" t="str">
+      <c r="K4" t="str">
         <v>50.00</v>
       </c>
-      <c r="I4" s="1">
+      <c r="L4" s="1">
         <v>45069.645949074074</v>
       </c>
     </row>
@@ -547,6 +583,15 @@
       <c r="I5" s="1">
         <v>45069.645949074074</v>
       </c>
+      <c r="J5" t="str">
+        <v>supplier_3</v>
+      </c>
+      <c r="K5" t="str">
+        <v>10.00</v>
+      </c>
+      <c r="L5" s="1">
+        <v>45069.645949074074</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -568,12 +613,21 @@
         <v>45100.645949074074</v>
       </c>
       <c r="G6" t="str">
+        <v/>
+      </c>
+      <c r="H6" t="str">
+        <v/>
+      </c>
+      <c r="I6" t="str">
+        <v/>
+      </c>
+      <c r="J6" t="str">
         <v>supplier_3</v>
       </c>
-      <c r="H6" t="str">
+      <c r="K6" t="str">
         <v>100.00</v>
       </c>
-      <c r="I6" s="1">
+      <c r="L6" s="1">
         <v>45100.645949074074</v>
       </c>
     </row>
@@ -597,18 +651,27 @@
         <v>45100.645949074074</v>
       </c>
       <c r="G7" t="str">
+        <v/>
+      </c>
+      <c r="H7" t="str">
+        <v/>
+      </c>
+      <c r="I7" t="str">
+        <v/>
+      </c>
+      <c r="J7" t="str">
         <v>supplier_3</v>
       </c>
-      <c r="H7" t="str">
+      <c r="K7" t="str">
         <v>10.00</v>
       </c>
-      <c r="I7" s="1">
+      <c r="L7" s="1">
         <v>45100.645949074074</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented product search functionality for price tracking
</commit_message>
<xml_diff>
--- a/excel_sheets/output.xlsx
+++ b/excel_sheets/output.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -432,13 +432,13 @@
         <v>Prev Supplier Date</v>
       </c>
       <c r="J1" t="str">
-        <v>Minimum Supplier Name</v>
+        <v>Minimum Overall Supplier Name</v>
       </c>
       <c r="K1" t="str">
-        <v>Minimum Supplier Unit Price</v>
+        <v>Minimum Overall Supplier Unit Price</v>
       </c>
       <c r="L1" t="str">
-        <v>Minimum Supplier Date</v>
+        <v>Minimum Overall Supplier Date</v>
       </c>
     </row>
     <row r="2">
@@ -481,37 +481,37 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B3" t="str">
-        <v>cabbiage</v>
+        <v>rice</v>
       </c>
       <c r="C3" t="str">
-        <v>1.00</v>
+        <v>11.00</v>
       </c>
       <c r="D3" t="str">
-        <v>supplier_1</v>
+        <v>supplier_3</v>
       </c>
       <c r="E3" t="str">
         <v>50.00</v>
       </c>
       <c r="F3" s="1">
+        <v>45100.645949074074</v>
+      </c>
+      <c r="G3" t="str">
+        <v>supplier_3</v>
+      </c>
+      <c r="H3" t="str">
+        <v>10.00</v>
+      </c>
+      <c r="I3" s="1">
         <v>45069.645949074074</v>
       </c>
-      <c r="G3" t="str">
-        <v/>
-      </c>
-      <c r="H3" t="str">
-        <v/>
-      </c>
-      <c r="I3" t="str">
-        <v/>
-      </c>
       <c r="J3" t="str">
-        <v>supplier_1</v>
+        <v>supplier_3</v>
       </c>
       <c r="K3" t="str">
-        <v>50.00</v>
+        <v>10.00</v>
       </c>
       <c r="L3" s="1">
         <v>45069.645949074074</v>
@@ -519,22 +519,22 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B4" t="str">
-        <v>onion</v>
+        <v>white rice</v>
       </c>
       <c r="C4" t="str">
         <v>1.00</v>
       </c>
       <c r="D4" t="str">
-        <v>supplier_1</v>
+        <v>supplier_3</v>
       </c>
       <c r="E4" t="str">
-        <v>50.00</v>
+        <v>100.00</v>
       </c>
       <c r="F4" s="1">
-        <v>45069.645949074074</v>
+        <v>45100.645949074074</v>
       </c>
       <c r="G4" t="str">
         <v/>
@@ -546,42 +546,42 @@
         <v/>
       </c>
       <c r="J4" t="str">
-        <v>supplier_1</v>
+        <v>supplier_3</v>
       </c>
       <c r="K4" t="str">
-        <v>50.00</v>
+        <v>100.00</v>
       </c>
       <c r="L4" s="1">
-        <v>45069.645949074074</v>
+        <v>45100.645949074074</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B5" t="str">
-        <v>rice</v>
+        <v>brown rice</v>
       </c>
       <c r="C5" t="str">
-        <v>11.00</v>
+        <v>5.00</v>
       </c>
       <c r="D5" t="str">
         <v>supplier_3</v>
       </c>
       <c r="E5" t="str">
-        <v>50.00</v>
+        <v>10.00</v>
       </c>
       <c r="F5" s="1">
         <v>45100.645949074074</v>
       </c>
       <c r="G5" t="str">
-        <v>supplier_3</v>
+        <v/>
       </c>
       <c r="H5" t="str">
-        <v>10.00</v>
-      </c>
-      <c r="I5" s="1">
-        <v>45069.645949074074</v>
+        <v/>
+      </c>
+      <c r="I5" t="str">
+        <v/>
       </c>
       <c r="J5" t="str">
         <v>supplier_3</v>
@@ -590,88 +590,12 @@
         <v>10.00</v>
       </c>
       <c r="L5" s="1">
-        <v>45069.645949074074</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6">
-        <v>21</v>
-      </c>
-      <c r="B6" t="str">
-        <v>white rice</v>
-      </c>
-      <c r="C6" t="str">
-        <v>1.00</v>
-      </c>
-      <c r="D6" t="str">
-        <v>supplier_3</v>
-      </c>
-      <c r="E6" t="str">
-        <v>100.00</v>
-      </c>
-      <c r="F6" s="1">
-        <v>45100.645949074074</v>
-      </c>
-      <c r="G6" t="str">
-        <v/>
-      </c>
-      <c r="H6" t="str">
-        <v/>
-      </c>
-      <c r="I6" t="str">
-        <v/>
-      </c>
-      <c r="J6" t="str">
-        <v>supplier_3</v>
-      </c>
-      <c r="K6" t="str">
-        <v>100.00</v>
-      </c>
-      <c r="L6" s="1">
-        <v>45100.645949074074</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7">
-        <v>22</v>
-      </c>
-      <c r="B7" t="str">
-        <v>brown rice</v>
-      </c>
-      <c r="C7" t="str">
-        <v>5.00</v>
-      </c>
-      <c r="D7" t="str">
-        <v>supplier_3</v>
-      </c>
-      <c r="E7" t="str">
-        <v>10.00</v>
-      </c>
-      <c r="F7" s="1">
-        <v>45100.645949074074</v>
-      </c>
-      <c r="G7" t="str">
-        <v/>
-      </c>
-      <c r="H7" t="str">
-        <v/>
-      </c>
-      <c r="I7" t="str">
-        <v/>
-      </c>
-      <c r="J7" t="str">
-        <v>supplier_3</v>
-      </c>
-      <c r="K7" t="str">
-        <v>10.00</v>
-      </c>
-      <c r="L7" s="1">
         <v>45100.645949074074</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Chaned the promise utilization in the for loop to await statement
</commit_message>
<xml_diff>
--- a/excel_sheets/output.xlsx
+++ b/excel_sheets/output.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -481,37 +481,37 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="B3" t="str">
-        <v>rice</v>
+        <v>cabbiage</v>
       </c>
       <c r="C3" t="str">
-        <v>11.00</v>
+        <v>1.00</v>
       </c>
       <c r="D3" t="str">
-        <v>supplier_3</v>
+        <v>supplier_1</v>
       </c>
       <c r="E3" t="str">
         <v>50.00</v>
       </c>
       <c r="F3" s="1">
-        <v>45100.645949074074</v>
+        <v>45069.645949074074</v>
       </c>
       <c r="G3" t="str">
-        <v>supplier_3</v>
+        <v/>
       </c>
       <c r="H3" t="str">
-        <v>10.00</v>
-      </c>
-      <c r="I3" s="1">
-        <v>45069.645949074074</v>
+        <v/>
+      </c>
+      <c r="I3" t="str">
+        <v/>
       </c>
       <c r="J3" t="str">
-        <v>supplier_3</v>
+        <v>supplier_1</v>
       </c>
       <c r="K3" t="str">
-        <v>10.00</v>
+        <v>50.00</v>
       </c>
       <c r="L3" s="1">
         <v>45069.645949074074</v>
@@ -519,22 +519,22 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" t="str">
-        <v>white rice</v>
+        <v>onion</v>
       </c>
       <c r="C4" t="str">
         <v>1.00</v>
       </c>
       <c r="D4" t="str">
-        <v>supplier_3</v>
+        <v>supplier_1</v>
       </c>
       <c r="E4" t="str">
-        <v>100.00</v>
+        <v>50.00</v>
       </c>
       <c r="F4" s="1">
-        <v>45100.645949074074</v>
+        <v>45069.645949074074</v>
       </c>
       <c r="G4" t="str">
         <v/>
@@ -546,42 +546,42 @@
         <v/>
       </c>
       <c r="J4" t="str">
-        <v>supplier_3</v>
+        <v>supplier_1</v>
       </c>
       <c r="K4" t="str">
-        <v>100.00</v>
+        <v>50.00</v>
       </c>
       <c r="L4" s="1">
-        <v>45100.645949074074</v>
+        <v>45069.645949074074</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B5" t="str">
-        <v>brown rice</v>
+        <v>rice</v>
       </c>
       <c r="C5" t="str">
-        <v>5.00</v>
+        <v>11.00</v>
       </c>
       <c r="D5" t="str">
         <v>supplier_3</v>
       </c>
       <c r="E5" t="str">
-        <v>10.00</v>
+        <v>50.00</v>
       </c>
       <c r="F5" s="1">
         <v>45100.645949074074</v>
       </c>
       <c r="G5" t="str">
-        <v/>
+        <v>supplier_3</v>
       </c>
       <c r="H5" t="str">
-        <v/>
-      </c>
-      <c r="I5" t="str">
-        <v/>
+        <v>10.00</v>
+      </c>
+      <c r="I5" s="1">
+        <v>45069.645949074074</v>
       </c>
       <c r="J5" t="str">
         <v>supplier_3</v>
@@ -590,12 +590,88 @@
         <v>10.00</v>
       </c>
       <c r="L5" s="1">
+        <v>45069.645949074074</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>21</v>
+      </c>
+      <c r="B6" t="str">
+        <v>white rice</v>
+      </c>
+      <c r="C6" t="str">
+        <v>1.00</v>
+      </c>
+      <c r="D6" t="str">
+        <v>supplier_3</v>
+      </c>
+      <c r="E6" t="str">
+        <v>100.00</v>
+      </c>
+      <c r="F6" s="1">
+        <v>45100.645949074074</v>
+      </c>
+      <c r="G6" t="str">
+        <v/>
+      </c>
+      <c r="H6" t="str">
+        <v/>
+      </c>
+      <c r="I6" t="str">
+        <v/>
+      </c>
+      <c r="J6" t="str">
+        <v>supplier_3</v>
+      </c>
+      <c r="K6" t="str">
+        <v>100.00</v>
+      </c>
+      <c r="L6" s="1">
+        <v>45100.645949074074</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>22</v>
+      </c>
+      <c r="B7" t="str">
+        <v>brown rice</v>
+      </c>
+      <c r="C7" t="str">
+        <v>5.00</v>
+      </c>
+      <c r="D7" t="str">
+        <v>supplier_3</v>
+      </c>
+      <c r="E7" t="str">
+        <v>10.00</v>
+      </c>
+      <c r="F7" s="1">
+        <v>45100.645949074074</v>
+      </c>
+      <c r="G7" t="str">
+        <v/>
+      </c>
+      <c r="H7" t="str">
+        <v/>
+      </c>
+      <c r="I7" t="str">
+        <v/>
+      </c>
+      <c r="J7" t="str">
+        <v>supplier_3</v>
+      </c>
+      <c r="K7" t="str">
+        <v>10.00</v>
+      </c>
+      <c r="L7" s="1">
         <v>45100.645949074074</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>